<commit_message>
Replaced old version of research log
</commit_message>
<xml_diff>
--- a/Research-log.xlsx
+++ b/Research-log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\galax\Downloads\codes\3390 (App Dev)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1F6505-982D-4AD2-99A6-25BD6D7BD36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C63619-A0C9-42D0-BDD2-8C509E705F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>Code language</t>
   </si>
@@ -97,18 +97,6 @@
     <t>https://developer.mozilla.org/en-US/docs/Learn_web_development/Core/Frameworks_libraries/Vue_getting_started</t>
   </si>
   <si>
-    <t>https://vuejs.org/guide/quick-start.html</t>
-  </si>
-  <si>
-    <t>https://tailwindcss.com/docs/installation</t>
-  </si>
-  <si>
-    <t>https://tailwindcss.com/docs/utility-first</t>
-  </si>
-  <si>
-    <t>https://tailwindcss.com/docs/guides/vite</t>
-  </si>
-  <si>
     <t>https://www.freecodecamp.org/news/what-is-tailwind-css-a-beginners-guide/</t>
   </si>
   <si>
@@ -157,18 +145,6 @@
     <t>MDN getting started with Vue, including setup and first app.</t>
   </si>
   <si>
-    <t>Vue quick start with Vite and single-file components.</t>
-  </si>
-  <si>
-    <t>Official Tailwind installation guide (including Vite, PostCSS).</t>
-  </si>
-  <si>
-    <t>Explains Tailwind’s utility-first approach and how to style in markup.</t>
-  </si>
-  <si>
-    <t>Official guide: set up Tailwind in a Vite project (works great with React/Vue/Svelte).</t>
-  </si>
-  <si>
     <t>Beginner-friendly overview of Tailwind’s concepts and benefits.</t>
   </si>
   <si>
@@ -209,13 +185,37 @@
   </si>
   <si>
     <t>SvelteKit Introduction Course | Routes, Groups &amp; API Endpoints | Basic Lesson for Beginners</t>
+  </si>
+  <si>
+    <t>Javascript</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/JavaScript/Guide/Modules</t>
+  </si>
+  <si>
+    <t>guide gives you all you need to get started with JavaScript module syntax</t>
+  </si>
+  <si>
+    <t>sveltejs/svelte: web development for the rest of us</t>
+  </si>
+  <si>
+    <t>Svelte Github Repository with quick reference links</t>
+  </si>
+  <si>
+    <t>https://tailwindcss.com/docs</t>
+  </si>
+  <si>
+    <t>Official Tailwind documentation for free version</t>
+  </si>
+  <si>
+    <t>YouTube account that has multiple videos with guides and tutorials about Svelte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +247,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0F0F0F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -291,7 +298,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -301,6 +308,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -609,19 +618,19 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="106.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="110.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,7 +647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -646,13 +655,16 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -660,13 +672,16 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -674,13 +689,16 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -688,13 +706,16 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -702,245 +723,296 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3.472222222222222E-3</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
+        <v>56</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3.125E-2</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>33</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2.2916666666666665E-2</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="D11" s="5">
+        <v>3.4722222222222224E-2</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="5">
+        <v>4.2361111111111113E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="5">
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="E16" t="s">
         <v>42</v>
       </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2.2916666666666665E-2</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="D18" s="5">
+        <v>2.4305555555555556E-2</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>61</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>59</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>62</v>
+      </c>
+      <c r="D23" s="5">
+        <v>6.25E-2</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -950,22 +1022,23 @@
     <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B13" r:id="rId21" xr:uid="{22551915-830B-4E7E-896E-08547E4AD8F0}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B14" r:id="rId18" xr:uid="{22551915-830B-4E7E-896E-08547E4AD8F0}"/>
+    <hyperlink ref="B7" r:id="rId19" xr:uid="{75134964-7B33-4F04-998F-5DC290C0B570}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://github.com/sveltejs/svelte" xr:uid="{2CE29931-6EE6-4EDA-8E17-3703C0E76D78}"/>
+    <hyperlink ref="B15" r:id="rId21" xr:uid="{4736F8A5-4833-49EB-84F1-A244434AB3B7}"/>
+    <hyperlink ref="B23" r:id="rId22" display="https://www.youtube.com/@SlateDevelopment" xr:uid="{BD269B73-61B1-4C17-9FDB-544723344BDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>